<commit_message>
Solución Fecha de registro
</commit_message>
<xml_diff>
--- a/00_Documentacion/prematriculas.xlsx
+++ b/00_Documentacion/prematriculas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jclah\Desktop\DAW\Programacion\Proyecto-DAW\00_Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD17EAF1-7E77-4849-8E3F-DFB391BFFCFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12C34B8-1ABD-4477-B4C2-CF0C6EB21F81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D11E7EE6-D704-40AA-84C1-2C77837DD476}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D11E7EE6-D704-40AA-84C1-2C77837DD476}"/>
   </bookViews>
   <sheets>
     <sheet name="Filtro" sheetId="1" r:id="rId1"/>
@@ -648,18 +648,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -675,17 +674,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Entrada" xfId="2" builtinId="20"/>
@@ -1928,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18754FFD-0C2E-4F29-91CF-657207021717}">
   <dimension ref="A1:BL26"/>
   <sheetViews>
-    <sheetView topLeftCell="AW1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:BL9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1948,88 +1948,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22" t="s">
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22" t="s">
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
       <c r="V1" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="W1" s="23" t="s">
+      <c r="W1" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="23" t="s">
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="26" t="s">
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="30" t="s">
+      <c r="AN1" s="34"/>
+      <c r="AO1" s="34"/>
+      <c r="AP1" s="34"/>
+      <c r="AQ1" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="31"/>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="32"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22"/>
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
+      <c r="AY1" s="22"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22"/>
+      <c r="BG1" s="22"/>
+      <c r="BH1" s="22"/>
+      <c r="BI1" s="22"/>
+      <c r="BJ1" s="22"/>
+      <c r="BK1" s="22"/>
+      <c r="BL1" s="23"/>
     </row>
     <row r="2" spans="1:64" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
@@ -2420,24 +2420,24 @@
       </c>
     </row>
     <row r="4" spans="1:64" ht="15" x14ac:dyDescent="0.25">
-      <c r="AW4" s="34" t="s">
+      <c r="AW4" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="AX4" s="34"/>
-      <c r="AY4" s="34"/>
-      <c r="AZ4" s="35" t="s">
+      <c r="AX4" s="25"/>
+      <c r="AY4" s="25"/>
+      <c r="AZ4" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="BA4" s="35"/>
-      <c r="BB4" s="35"/>
+      <c r="BA4" s="26"/>
+      <c r="BB4" s="26"/>
       <c r="BC4" s="1"/>
       <c r="BD4" s="1"/>
       <c r="BE4" s="1"/>
-      <c r="BF4" s="33" t="s">
+      <c r="BF4" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="BG4" s="33"/>
-      <c r="BH4" s="33"/>
+      <c r="BG4" s="24"/>
+      <c r="BH4" s="24"/>
       <c r="BI4" s="2"/>
       <c r="BJ4" s="2"/>
       <c r="BK4" s="2"/>
@@ -2612,13 +2612,13 @@
         <f>IF('[1]Respuestas de formulario 1'!BN1="","",'[1]Respuestas de formulario 1'!BN1)</f>
         <v>Código postal</v>
       </c>
-      <c r="AQ5" s="36" t="s">
+      <c r="AQ5" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="AR5" s="37"/>
-      <c r="AS5" s="37"/>
-      <c r="AT5" s="38"/>
-      <c r="AU5" s="38"/>
+      <c r="AR5" s="28"/>
+      <c r="AS5" s="28"/>
+      <c r="AT5" s="29"/>
+      <c r="AU5" s="29"/>
       <c r="AV5" s="3" t="str">
         <f>IF('[1]Respuestas de formulario 1'!BO1="","",'[1]Respuestas de formulario 1'!BO1)</f>
         <v>Opción de 1º Bachillerato</v>
@@ -4806,11 +4806,11 @@
       <c r="AW14" s="1"/>
       <c r="AX14" s="1"/>
       <c r="AY14" s="1"/>
-      <c r="AZ14" s="33" t="s">
+      <c r="AZ14" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="BA14" s="33"/>
-      <c r="BB14" s="33"/>
+      <c r="BA14" s="24"/>
+      <c r="BB14" s="24"/>
       <c r="BC14" t="str">
         <f>IF('[1]Respuestas de formulario 1'!BY10="","",'[1]Respuestas de formulario 1'!BY10)</f>
         <v/>
@@ -5277,7 +5277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5AFCBA7-8426-4CF7-867F-A2A0F6C340DD}">
   <dimension ref="A3:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D25" sqref="D25:D40"/>
     </sheetView>
   </sheetViews>
@@ -5616,7 +5616,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="19" t="s">
         <v>102</v>
       </c>
       <c r="B25" t="s">
@@ -5631,7 +5631,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="19" t="s">
         <v>103</v>
       </c>
       <c r="B26" t="s">
@@ -5646,7 +5646,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="19" t="s">
         <v>104</v>
       </c>
       <c r="B27" t="s">
@@ -5661,7 +5661,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="19" t="s">
         <v>105</v>
       </c>
       <c r="B28" t="s">
@@ -5676,7 +5676,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="19" t="s">
         <v>106</v>
       </c>
       <c r="B29" t="s">
@@ -5691,7 +5691,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="19" t="s">
         <v>46</v>
       </c>
       <c r="B30" t="s">
@@ -5706,7 +5706,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="20" t="s">
         <v>107</v>
       </c>
       <c r="B31" t="s">
@@ -5721,7 +5721,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="20" t="s">
         <v>108</v>
       </c>
       <c r="B32" t="s">
@@ -5736,7 +5736,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="20" t="s">
         <v>109</v>
       </c>
       <c r="B33" t="s">
@@ -5751,7 +5751,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="20" t="s">
         <v>99</v>
       </c>
       <c r="B34" t="s">
@@ -5766,7 +5766,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="20" t="s">
         <v>100</v>
       </c>
       <c r="B35" t="s">
@@ -5781,7 +5781,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="20" t="s">
         <v>101</v>
       </c>
       <c r="B36" t="s">

</xml_diff>